<commit_message>
Resolved the Date Bug
</commit_message>
<xml_diff>
--- a/Temperature_VS_Time.xlsx
+++ b/Temperature_VS_Time.xlsx
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>18/2/2024, 7:05:51 pm IST</t>
+  </si>
+  <si>
+    <t>19/2/2024, 12:44:37 am IST</t>
+  </si>
+  <si>
+    <t>19/2/2024, 2:02:09 pm IST</t>
   </si>
 </sst>
 </file>
@@ -780,6 +786,28 @@
         <v>235.06862</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52">
+        <v>270.68928</v>
+      </c>
+      <c r="C52">
+        <v>270.49391</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53">
+        <v>116.83392</v>
+      </c>
+      <c r="C53">
+        <v>115.39074</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>